<commit_message>
programme principale + makefile
</commit_message>
<xml_diff>
--- a/CSV/Moyenne des algos resultatss.xlsx
+++ b/CSV/Moyenne des algos resultatss.xlsx
@@ -8,36 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\remy\ocaml\M1_Projet_ocaml\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B62F11-F772-4CCF-8A99-B77DB7659333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FEE715-688F-42FC-866C-816E2E0BEF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7925C184-6962-4BC9-8B6B-C0FF88B83616}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$A$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$A$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Feuil1!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Feuil1!$B$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Feuil1!$B$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Feuil1!$B$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Feuil1!$B$5:$F$5</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Feuil1!$B$6:$F$6</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Feuil1!$B$7:$F$7</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Feuil1!$B$8:$F$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$A$12</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Feuil1!$B$9:$F$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$A$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$A$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$A$5</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$A$6</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$A$7</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$A$8</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$A$9</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>taille</t>
   </si>
@@ -138,12 +115,15 @@
   <si>
     <t>6.78125</t>
   </si>
+  <si>
+    <t>CE FICHIER N'EST PAS MIS A JOUR A CHAQUE LANCEMENT DU PROGRAMME, IL A ÉTÉ REMPLIE A LA MAIN AVEC LES DONNEES QUE DONNE LE PROGRAMME P3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +133,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -252,7 +241,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$23</c:f>
+              <c:f>Feuil1!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -275,7 +264,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -313,7 +302,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$23:$K$23</c:f>
+              <c:f>Feuil1!$B$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -362,7 +351,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$24</c:f>
+              <c:f>Feuil1!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -385,7 +374,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -423,7 +412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$24:$K$24</c:f>
+              <c:f>Feuil1!$B$25:$K$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -472,7 +461,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$25</c:f>
+              <c:f>Feuil1!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -495,7 +484,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -533,7 +522,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$25:$K$25</c:f>
+              <c:f>Feuil1!$B$26:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -582,7 +571,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$26</c:f>
+              <c:f>Feuil1!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -605,7 +594,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -643,7 +632,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$26:$K$26</c:f>
+              <c:f>Feuil1!$B$27:$K$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -692,7 +681,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$27</c:f>
+              <c:f>Feuil1!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -715,7 +704,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -753,7 +742,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$27:$K$27</c:f>
+              <c:f>Feuil1!$B$28:$K$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -802,7 +791,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$28</c:f>
+              <c:f>Feuil1!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -825,7 +814,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -863,7 +852,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$28:$K$28</c:f>
+              <c:f>Feuil1!$B$29:$K$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -912,7 +901,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$29</c:f>
+              <c:f>Feuil1!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -937,7 +926,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -975,7 +964,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$29:$K$29</c:f>
+              <c:f>Feuil1!$B$30:$K$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1024,7 +1013,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$30</c:f>
+              <c:f>Feuil1!$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1049,7 +1038,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1087,7 +1076,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$30:$K$30</c:f>
+              <c:f>Feuil1!$B$31:$K$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1136,7 +1125,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$31</c:f>
+              <c:f>Feuil1!$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1161,7 +1150,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1199,7 +1188,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$31:$K$31</c:f>
+              <c:f>Feuil1!$B$32:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1248,7 +1237,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$32</c:f>
+              <c:f>Feuil1!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1273,7 +1262,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1311,7 +1300,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$32:$K$32</c:f>
+              <c:f>Feuil1!$B$33:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1360,7 +1349,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$33</c:f>
+              <c:f>Feuil1!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1385,7 +1374,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$22:$K$22</c:f>
+              <c:f>Feuil1!$B$23:$K$23</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1423,7 +1412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$33:$K$33</c:f>
+              <c:f>Feuil1!$B$34:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1717,7 +1706,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$2</c:f>
+              <c:f>Feuil1!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1740,7 +1729,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$3:$A$13</c:f>
+              <c:f>Feuil1!$A$4:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1781,7 +1770,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$3:$B$13</c:f>
+              <c:f>Feuil1!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1833,7 +1822,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$2</c:f>
+              <c:f>Feuil1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1856,7 +1845,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$3:$A$13</c:f>
+              <c:f>Feuil1!$A$4:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1897,7 +1886,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$3:$C$13</c:f>
+              <c:f>Feuil1!$C$4:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1949,7 +1938,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$2</c:f>
+              <c:f>Feuil1!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1972,7 +1961,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$3:$A$13</c:f>
+              <c:f>Feuil1!$A$4:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -2013,7 +2002,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$3:$D$13</c:f>
+              <c:f>Feuil1!$D$4:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2065,7 +2054,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$2</c:f>
+              <c:f>Feuil1!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2088,7 +2077,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$3:$A$13</c:f>
+              <c:f>Feuil1!$A$4:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -2129,7 +2118,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$3:$E$13</c:f>
+              <c:f>Feuil1!$E$4:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2181,7 +2170,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$F$2</c:f>
+              <c:f>Feuil1!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2204,7 +2193,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$3:$A$13</c:f>
+              <c:f>Feuil1!$A$4:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -2245,7 +2234,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$F$3:$F$13</c:f>
+              <c:f>Feuil1!$F$4:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3612,13 +3601,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3648,13 +3637,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3980,10 +3969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F9189E-05A3-48E0-8B71-1A779020B133}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="A22:K33"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3992,60 +3981,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
+      <c r="A1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <f>AVERAGE(B3:F3)</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4063,13 +4033,13 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G13" si="0">AVERAGE(B4:F4)</f>
+        <f>AVERAGE(B4:F4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4087,13 +4057,13 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G5:G14" si="0">AVERAGE(B5:F5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4117,7 +4087,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4141,7 +4111,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4153,19 +4123,19 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1250000000000002E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4177,46 +4147,46 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.1250000000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -4225,149 +4195,134 @@
         <v>1.5625E-2</v>
       </c>
       <c r="E11">
-        <v>1.5625E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F11">
         <v>1.5625E-2</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>9.3749999999999997E-3</v>
+        <v>1.5625E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>0.265625</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0.671875</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="E12">
-        <v>1.078125</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="F12">
-        <v>0.78125</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>0.57187500000000002</v>
+        <v>9.3749999999999997E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>52.796875</v>
+        <v>0.265625</v>
       </c>
       <c r="C13">
-        <v>8.140625</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D13">
-        <v>113.48478799999999</v>
+        <v>0.671875</v>
       </c>
       <c r="E13">
-        <v>165.640625</v>
+        <v>1.078125</v>
       </c>
       <c r="F13">
-        <v>57.859372999999998</v>
+        <v>0.78125</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
+        <v>0.57187500000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>52.796875</v>
+      </c>
+      <c r="C14">
+        <v>8.140625</v>
+      </c>
+      <c r="D14">
+        <v>113.48478799999999</v>
+      </c>
+      <c r="E14">
+        <v>165.640625</v>
+      </c>
+      <c r="F14">
+        <v>57.859372999999998</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
         <v>79.584457200000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <f>AVERAGE(B23:K23)</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -4397,16 +4352,16 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L33" si="1">AVERAGE(B24:K24)</f>
-        <v>1.5625000000000001E-3</v>
+        <f>AVERAGE(B24:K24)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4436,16 +4391,16 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="L25:L34" si="1">AVERAGE(B25:K25)</f>
+        <v>1.5625000000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4484,7 +4439,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4502,7 +4457,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -4518,12 +4473,12 @@
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>1.5625000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4541,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1.5625E-2</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -4557,12 +4512,12 @@
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5625000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4601,13 +4556,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4635,24 +4590,24 @@
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>1.5625000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
         <v>1.5625E-2</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -4661,7 +4616,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>1.5625E-2</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -4674,12 +4629,12 @@
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>6.2500000000000003E-3</v>
+        <v>1.5625000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32">
         <v>1.5625E-2</v>
@@ -4688,69 +4643,108 @@
         <v>0</v>
       </c>
       <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>1.5625E-2</v>
       </c>
-      <c r="E32">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="F32">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="G32">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>1.7187500000000001E-2</v>
+        <v>6.2500000000000003E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="E33">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="F33">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G33">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K33">
+        <v>6.25E-2</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>1.7187500000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>11</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>0.234375</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>1.03125</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>0.125</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>1.328125</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>0.1875</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G34" t="s">
         <v>25</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <v>7.8125E-2</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>3.125E-2</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>6.25E-2</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>1.234375</v>
       </c>
-      <c r="L33">
+      <c r="L34">
         <f t="shared" si="1"/>
         <v>0.47916666666666669</v>
       </c>

</xml_diff>